<commit_message>
update anova and regression
</commit_message>
<xml_diff>
--- a/biostat project.xlsx
+++ b/biostat project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\biostat project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mphcmiuedu-my.sharepoint.com/personal/btariu16021_student_hcmiu_edu_vn/Documents/Documents/GitHub/Biostatistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C196E0-1F1F-4AA4-9ECD-50D0348CEE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:1_{03C196E0-1F1F-4AA4-9ECD-50D0348CEE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{719A32A2-B009-445A-891D-D26B5B8A3A87}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="9" xr2:uid="{AC73E270-B892-4892-9C6E-FCD3E64DCA84}"/>
   </bookViews>
@@ -21,8 +21,8 @@
     <sheet name="1 pop proportion test" sheetId="6" r:id="rId6"/>
     <sheet name="1 pop var test" sheetId="7" r:id="rId7"/>
     <sheet name="2 mean test" sheetId="8" r:id="rId8"/>
-    <sheet name="Anova" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
+    <sheet name="Anova-1-way" sheetId="10" r:id="rId9"/>
+    <sheet name="Regression" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="322">
   <si>
     <t>Ex 1:</t>
   </si>
@@ -782,135 +782,33 @@
     <t>Conclusion: There was a difference in mean fatigue between men and women when working at 16oC</t>
   </si>
   <si>
-    <t xml:space="preserve">Exercise 1:The presence of harmful insects in farm fields is detected by erecting boards which are covered  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The table below gives the numbers of cereal leaf beetles trapped. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">To investigate which colours are most attractive to cereal leaf beetles researchers placed six boards of each of four colours in a field of oats in July. </t>
-  </si>
-  <si>
-    <t>with a sticky material and then examining the insects trapped on the board.</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Lemon Yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green </t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Insects trapped</t>
-  </si>
-  <si>
-    <t>Does this data suggest that colour influences the number of beetles?   </t>
-  </si>
-  <si>
-    <t>H_0: Mean abundance is the same for all colours of boards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H_1: At least one pair of means differ </t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
     <t>Error Deviation</t>
   </si>
   <si>
     <t>Error Deviation ^2</t>
   </si>
   <si>
-    <t>Grandmean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSE </t>
-  </si>
-  <si>
-    <t>MSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n </t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>SSTr</t>
   </si>
   <si>
-    <t>n_1</t>
-  </si>
-  <si>
-    <t>n_2</t>
-  </si>
-  <si>
-    <t>n_3</t>
-  </si>
-  <si>
-    <t>n_4</t>
-  </si>
-  <si>
-    <t>MSTr</t>
-  </si>
-  <si>
     <t>F_score</t>
   </si>
   <si>
-    <t>F_critical</t>
-  </si>
-  <si>
     <t>Since F_score &gt; F_crit</t>
   </si>
   <si>
     <t>Reject Ho</t>
   </si>
   <si>
-    <t>Conclusion: There were significant differences amanong mean abundance</t>
-  </si>
-  <si>
-    <t>Anova: Single Factor</t>
-  </si>
-  <si>
-    <t>SUMMARY</t>
-  </si>
-  <si>
-    <t>Groups</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
     <t>Variance</t>
   </si>
   <si>
     <t>ANOVA</t>
   </si>
   <si>
-    <t>Source of Variation</t>
-  </si>
-  <si>
     <t>SS</t>
   </si>
   <si>
@@ -924,15 +822,6 @@
   </si>
   <si>
     <t>P-value</t>
-  </si>
-  <si>
-    <t>F crit</t>
-  </si>
-  <si>
-    <t>Between Groups</t>
-  </si>
-  <si>
-    <t>Within Groups</t>
   </si>
   <si>
     <t>Total</t>
@@ -1065,6 +954,138 @@
   <si>
     <t>ChiSquare Score =</t>
   </si>
+  <si>
+    <t>ANOVA TEST</t>
+  </si>
+  <si>
+    <t>Grand mean</t>
+  </si>
+  <si>
+    <t>SSE</t>
+  </si>
+  <si>
+    <t>MSE = SSE/(n-r)</t>
+  </si>
+  <si>
+    <t>n = 25</t>
+  </si>
+  <si>
+    <t>r (# groups) =3</t>
+  </si>
+  <si>
+    <t>MSTr = SSTr/(r-1)</t>
+  </si>
+  <si>
+    <t>F_score = MSTr/MSE</t>
+  </si>
+  <si>
+    <t>F_crit</t>
+  </si>
+  <si>
+    <t>Conclusion: There is evidence of significant differences among the treatment mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise 1: The table below gives the estimated world population (in billions) for various </t>
+  </si>
+  <si>
+    <t>Using the linear regression equation predict the world population in the year 2015.</t>
+  </si>
+  <si>
+    <t>Year (X)</t>
+  </si>
+  <si>
+    <t>Population (Y)</t>
+  </si>
+  <si>
+    <t>X - Xbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y -Ybar </t>
+  </si>
+  <si>
+    <t>(X-Xbar)^2</t>
+  </si>
+  <si>
+    <t>(Y-Ybar)^2</t>
+  </si>
+  <si>
+    <t>(X-Xbar)*(Y-Ybar)</t>
+  </si>
+  <si>
+    <t>SSx</t>
+  </si>
+  <si>
+    <t>Ssxy</t>
+  </si>
+  <si>
+    <t>SSy</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>X Variable 1</t>
+  </si>
+  <si>
+    <t>b0 = y_bar - b1*X_bar</t>
+  </si>
+  <si>
+    <t>b1 = Ssxy/SSx</t>
+  </si>
+  <si>
+    <t>R = Ssxy/(SSx * Ssy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R^2 </t>
+  </si>
 </sst>
 </file>
 
@@ -1074,7 +1095,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1121,15 +1142,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.5"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -1189,7 +1204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1410,30 +1425,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1470,7 +1461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1536,29 +1527,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1646,14 +1625,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1995,11 +1974,11 @@
       <c r="B2" s="16"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="11" t="s">
@@ -2040,11 +2019,11 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="64"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="11" t="s">
@@ -2131,11 +2110,11 @@
       <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="B27" s="65" t="s">
+      <c r="B27" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="67"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="59"/>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="11" t="s">
@@ -2174,10 +2153,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="B35" s="20"/>
-      <c r="C35" s="68" t="s">
+      <c r="C35" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="68"/>
+      <c r="D35" s="60"/>
     </row>
     <row r="36" spans="1:4">
       <c r="B36" s="21" t="s">
@@ -2214,10 +2193,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="B40" s="20"/>
-      <c r="C40" s="68" t="s">
+      <c r="C40" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="68"/>
+      <c r="D40" s="60"/>
     </row>
     <row r="41" spans="1:4">
       <c r="B41" s="21" t="s">
@@ -2272,11 +2251,11 @@
       </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="57"/>
-      <c r="D49" s="58"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="50"/>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" s="11" t="s">
@@ -2493,524 +2472,488 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8BFC71-637A-402C-908B-044747BF6BC6}">
-  <dimension ref="B2:U30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AF2414-8DDF-4A2C-96A8-716BB84515E9}">
+  <dimension ref="A2:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21:U21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21">
-      <c r="B2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21">
-      <c r="B3" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21">
-      <c r="C5" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>287</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="H5" s="87" t="s">
+    <row r="2" spans="1:15">
+      <c r="B2" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="N5" s="81" t="s">
+    </row>
+    <row r="3" spans="1:15">
+      <c r="B3" s="79" t="s">
+        <v>289</v>
+      </c>
+      <c r="J3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E4" t="s">
+        <v>293</v>
+      </c>
+      <c r="F4" t="s">
+        <v>294</v>
+      </c>
+      <c r="G4" t="s">
+        <v>295</v>
+      </c>
+      <c r="H4" t="s">
         <v>296</v>
       </c>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="C6" s="35">
-        <v>7</v>
-      </c>
-      <c r="D6" s="35">
-        <v>11</v>
-      </c>
-      <c r="E6" s="35">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>289</v>
-      </c>
-      <c r="N6" s="35">
-        <v>7</v>
-      </c>
-      <c r="P6" t="s">
+    </row>
+    <row r="5" spans="1:15">
+      <c r="B5">
+        <v>1980</v>
+      </c>
+      <c r="C5">
+        <v>4400</v>
+      </c>
+      <c r="D5">
+        <f>B5-$B$12</f>
+        <v>-17.166666666666742</v>
+      </c>
+      <c r="E5">
+        <f>C5-$C$12</f>
+        <v>-1413.666666666667</v>
+      </c>
+      <c r="F5">
+        <f>D5^2</f>
+        <v>294.69444444444707</v>
+      </c>
+      <c r="G5">
+        <f>E5^2</f>
+        <v>1998453.4444444452</v>
+      </c>
+      <c r="H5">
+        <f>D5*E5</f>
+        <v>24267.944444444558</v>
+      </c>
+      <c r="J5" s="78" t="s">
+        <v>301</v>
+      </c>
+      <c r="K5" s="78"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="B6">
+        <v>1990</v>
+      </c>
+      <c r="C6">
+        <v>5100</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D10" si="0">B6-$B$12</f>
+        <v>-7.1666666666667425</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E10" si="1">C6-$C$12</f>
+        <v>-713.66666666666697</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F10" si="2">D6^2</f>
+        <v>51.361111111112194</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G10" si="3">E6^2</f>
+        <v>509320.11111111153</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H10" si="4">D6*E6</f>
+        <v>5114.6111111111677</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="K6" s="40">
+        <v>0.99802050280497323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="B7">
+        <v>1997</v>
+      </c>
+      <c r="C7">
+        <v>5852</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-0.16666666666674246</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>38.33333333333303</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>2.7777777777803041E-2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>1469.4444444444212</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>-6.3888888888917439</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="K7" s="40">
+        <v>0.99604492401909162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="B8">
+        <v>2000</v>
+      </c>
+      <c r="C8">
+        <v>6080</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2.8333333333332575</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>266.33333333333303</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>8.0277777777773487</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>70933.444444444278</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>754.61111111109005</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="K8" s="40">
+        <v>0.99505615502386457</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="B9">
+        <v>2005</v>
+      </c>
+      <c r="C9">
+        <v>6450</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>7.8333333333332575</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>636.33333333333303</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>61.361111111109921</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>404920.11111111072</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>4984.6111111110604</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="K9" s="40">
+        <v>65.902589721889143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B10">
+        <v>2011</v>
+      </c>
+      <c r="C10">
+        <v>7000</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>13.833333333333258</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>1186.333333333333</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>191.36111111110901</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>1407386.7777777771</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>16410.944444444351</v>
+      </c>
+      <c r="J10" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="K10" s="44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="F11" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="Q6">
-        <f>AVERAGE(N6:N30)</f>
-        <v>10.68</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21">
-      <c r="C7" s="36">
-        <v>12</v>
-      </c>
-      <c r="D7" s="36">
-        <v>17</v>
-      </c>
-      <c r="E7" s="36">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>290</v>
-      </c>
-      <c r="N7" s="36">
-        <v>12</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="G11" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="Q7">
-        <f>_xlfn.STDEV.S(N6:N30)</f>
-        <v>3.2496153618543846</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21">
-      <c r="C8" s="36">
-        <v>9</v>
-      </c>
-      <c r="D8" s="36">
-        <v>16</v>
-      </c>
-      <c r="E8" s="36">
-        <v>10</v>
-      </c>
-      <c r="H8" t="s">
-        <v>261</v>
-      </c>
-      <c r="I8">
-        <f>D17/C17</f>
-        <v>2.5854037267080727</v>
-      </c>
-      <c r="N8" s="36">
-        <v>9</v>
-      </c>
-      <c r="P8" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q8">
-        <f>_xlfn.NORM.INV(0.16,$Q$6,$Q$7)</f>
-        <v>7.448394386004404</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21">
-      <c r="C9" s="36">
-        <v>11</v>
-      </c>
-      <c r="D9" s="36">
-        <v>13</v>
-      </c>
-      <c r="E9" s="36">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>291</v>
-      </c>
-      <c r="I9">
-        <f>_xlfn.F.INV(0.025,D18 - 1, C18 - 1)</f>
-        <v>0.20733049797574626</v>
-      </c>
-      <c r="N9" s="36">
-        <v>11</v>
-      </c>
-      <c r="P9" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q9">
-        <f>_xlfn.NORM.INV(0.16 + 0.17,$Q$6,$Q$7)</f>
-        <v>9.2504514189462661</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21">
-      <c r="C10" s="36">
-        <v>8</v>
-      </c>
-      <c r="D10" s="36">
-        <v>10</v>
-      </c>
-      <c r="E10" s="36">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>292</v>
-      </c>
-      <c r="I10">
-        <f>_xlfn.F.INV(1 - 0.025,D18 - 1, C18 - 1)</f>
-        <v>4.1970466369455171</v>
-      </c>
-      <c r="N10" s="36">
-        <v>8</v>
-      </c>
-      <c r="P10" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q10">
-        <f>_xlfn.NORM.INV(0.16 + 0.17*2,$Q$6,$Q$7)</f>
-        <v>10.68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21">
-      <c r="C11" s="36">
-        <v>9</v>
-      </c>
-      <c r="D11" s="36">
-        <v>15</v>
-      </c>
-      <c r="E11" s="36">
-        <v>7</v>
-      </c>
-      <c r="H11" t="s">
-        <v>293</v>
-      </c>
-      <c r="N11" s="36">
-        <v>9</v>
-      </c>
-      <c r="P11" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q11">
-        <f>_xlfn.NORM.INV(0.16 + 0.17*3,$Q$6,$Q$7)</f>
-        <v>12.109548581053733</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21">
-      <c r="C12" s="36">
-        <v>11</v>
-      </c>
-      <c r="D12" s="36">
-        <v>14</v>
-      </c>
-      <c r="E12" s="36">
-        <v>10</v>
-      </c>
-      <c r="H12" t="s">
-        <v>294</v>
-      </c>
-      <c r="N12" s="36">
-        <v>11</v>
-      </c>
-      <c r="P12" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q12">
-        <f>_xlfn.NORM.INV(0.16 + 0.17*4,$Q$6,$Q$7)</f>
-        <v>13.911605613995604</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21">
-      <c r="C13" s="36">
-        <v>10</v>
-      </c>
-      <c r="D13" s="36">
-        <v>18</v>
-      </c>
-      <c r="E13" s="36"/>
-      <c r="H13" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="N13" s="36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21">
-      <c r="C14" s="36">
-        <v>7</v>
-      </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="N14" s="36">
-        <v>7</v>
-      </c>
-      <c r="R14" t="s">
-        <v>304</v>
-      </c>
-      <c r="S14" t="s">
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B5:B10)</f>
+        <v>1997.1666666666667</v>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(C5:C10)</f>
+        <v>5813.666666666667</v>
+      </c>
+      <c r="F12" s="16">
+        <f>SUM(F5:F10)</f>
+        <v>606.83333333333348</v>
+      </c>
+      <c r="G12" s="16">
+        <f>SUM(G5:G10)</f>
+        <v>4392483.333333334</v>
+      </c>
+      <c r="H12" s="16">
+        <f>SUM(H5:H10)</f>
+        <v>51526.333333333336</v>
+      </c>
+      <c r="J12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="F13" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="G13" s="16">
+        <f>H12/F12</f>
+        <v>84.910189508376803</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="L13" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="M13" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="N13" s="45" t="s">
+        <v>243</v>
+      </c>
+      <c r="O13" s="45" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="F14" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="G14" s="16">
+        <f>C12-G13*B12</f>
+        <v>-163766.13347981323</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="J14" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="K14" s="40">
+        <v>1</v>
+      </c>
+      <c r="L14" s="40">
+        <v>4375110.728005127</v>
+      </c>
+      <c r="M14" s="40">
+        <v>4375110.728005127</v>
+      </c>
+      <c r="N14" s="40">
+        <v>1007.358572960059</v>
+      </c>
+      <c r="O14" s="40">
+        <v>5.8737354777219821E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="F15" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="G15" s="16">
+        <f>H12/SQRT(F12*G12)</f>
+        <v>0.99802050280497323</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="J15" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="K15" s="40">
+        <v>4</v>
+      </c>
+      <c r="L15" s="40">
+        <v>17372.605328206591</v>
+      </c>
+      <c r="M15" s="40">
+        <v>4343.1513320516478</v>
+      </c>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1">
+      <c r="F16" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="G16" s="16">
+        <f>G15^2</f>
+        <v>0.99604492401909162</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="J16" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="K16" s="44">
+        <v>5</v>
+      </c>
+      <c r="L16" s="44">
+        <v>4392483.333333334</v>
+      </c>
+      <c r="M16" s="44"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+    </row>
+    <row r="17" spans="10:18" ht="15.75" thickBot="1"/>
+    <row r="18" spans="10:18">
+      <c r="J18" s="45"/>
+      <c r="K18" s="45" t="s">
+        <v>311</v>
+      </c>
+      <c r="L18" s="45" t="s">
         <v>305</v>
       </c>
-      <c r="T14" s="81" t="s">
-        <v>307</v>
-      </c>
-      <c r="U14" s="81"/>
-    </row>
-    <row r="15" spans="2:21">
-      <c r="C15" s="37">
-        <v>8</v>
-      </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="N15" s="36">
-        <v>8</v>
-      </c>
-      <c r="P15" s="81" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q15" s="81"/>
-      <c r="R15">
-        <f>COUNTIF(N6:N30,"&lt;"&amp;Q8)</f>
-        <v>4</v>
-      </c>
-      <c r="S15">
-        <f>D19*0.16</f>
-        <v>4</v>
-      </c>
-      <c r="T15" s="81">
-        <f>(R15-S15)^2/S15</f>
-        <v>0</v>
-      </c>
-      <c r="U15" s="81"/>
-    </row>
-    <row r="16" spans="2:21">
-      <c r="N16" s="36">
-        <v>11</v>
-      </c>
-      <c r="P16" s="81" t="s">
+      <c r="M18" s="45" t="s">
+        <v>312</v>
+      </c>
+      <c r="N18" s="45" t="s">
+        <v>244</v>
+      </c>
+      <c r="O18" s="45" t="s">
+        <v>313</v>
+      </c>
+      <c r="P18" s="45" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q18" s="45" t="s">
+        <v>315</v>
+      </c>
+      <c r="R18" s="45" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="10:18">
+      <c r="J19" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="Q16" s="81"/>
-      <c r="R16">
-        <f>COUNTIFS($N$6:$N$30,"&gt;"&amp;Q8,$N$6:$N$30,"&lt;"&amp;Q9)</f>
-        <v>6</v>
-      </c>
-      <c r="S16">
-        <f>$D$19*0.17</f>
-        <v>4.25</v>
-      </c>
-      <c r="T16" s="81">
-        <f t="shared" ref="T16:T20" si="0">(R16-S16)^2/S16</f>
-        <v>0.72058823529411764</v>
-      </c>
-      <c r="U16" s="81"/>
-    </row>
-    <row r="17" spans="2:21">
-      <c r="B17" t="s">
-        <v>271</v>
-      </c>
-      <c r="C17">
-        <f>_xlfn.VAR.S(C6:C15)</f>
-        <v>3.0666666666666691</v>
-      </c>
-      <c r="D17">
-        <f>_xlfn.VAR.S(D6:D13)</f>
-        <v>7.9285714285714288</v>
-      </c>
-      <c r="E17">
-        <f>_xlfn.VAR.S(E6:E12)</f>
-        <v>3.2380952380952408</v>
-      </c>
-      <c r="N17" s="36">
-        <v>17</v>
-      </c>
-      <c r="P17" s="81" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q17" s="81"/>
-      <c r="R17">
-        <f t="shared" ref="R17:R19" si="1">COUNTIFS($N$6:$N$30,"&gt;"&amp;Q9,$N$6:$N$30,"&lt;"&amp;Q10)</f>
-        <v>4</v>
-      </c>
-      <c r="S17">
-        <f t="shared" ref="S17:S19" si="2">$D$19*0.17</f>
-        <v>4.25</v>
-      </c>
-      <c r="T17" s="81">
-        <f t="shared" si="0"/>
-        <v>1.4705882352941176E-2</v>
-      </c>
-      <c r="U17" s="81"/>
-    </row>
-    <row r="18" spans="2:21">
-      <c r="B18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18">
-        <f>COUNT(C6:C15)</f>
-        <v>10</v>
-      </c>
-      <c r="D18">
-        <f t="shared" ref="D18:E18" si="3">COUNT(D6:D15)</f>
-        <v>8</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="N18" s="36">
-        <v>16</v>
-      </c>
-      <c r="P18" s="81" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q18" s="81"/>
-      <c r="R18">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="2"/>
-        <v>4.25</v>
-      </c>
-      <c r="T18" s="81">
-        <f t="shared" si="0"/>
-        <v>0.13235294117647059</v>
-      </c>
-      <c r="U18" s="81"/>
-    </row>
-    <row r="19" spans="2:21">
-      <c r="B19" s="81" t="s">
-        <v>306</v>
-      </c>
-      <c r="C19" s="81"/>
-      <c r="D19">
-        <f>SUM(C18:E18)</f>
-        <v>25</v>
-      </c>
-      <c r="N19" s="36">
-        <v>13</v>
-      </c>
-      <c r="P19" s="81" t="s">
-        <v>312</v>
-      </c>
-      <c r="Q19" s="81"/>
-      <c r="R19">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="2"/>
-        <v>4.25</v>
-      </c>
-      <c r="T19" s="81">
-        <f t="shared" si="0"/>
-        <v>2.4852941176470589</v>
-      </c>
-      <c r="U19" s="81"/>
-    </row>
-    <row r="20" spans="2:21">
-      <c r="N20" s="36">
-        <v>10</v>
-      </c>
-      <c r="P20" s="81" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q20" s="81"/>
-      <c r="R20">
-        <f>COUNTIF(N6:N30,"&gt;"&amp;Q12)</f>
-        <v>5</v>
-      </c>
-      <c r="S20">
-        <f>D19*0.16</f>
-        <v>4</v>
-      </c>
-      <c r="T20" s="81">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="U20" s="81"/>
-    </row>
-    <row r="21" spans="2:21">
-      <c r="N21" s="36">
-        <v>15</v>
-      </c>
-      <c r="R21" s="87" t="s">
-        <v>314</v>
-      </c>
-      <c r="S21" s="87"/>
-      <c r="T21" s="87">
-        <f>SUM(T15:U20)</f>
-        <v>3.6029411764705883</v>
-      </c>
-      <c r="U21" s="87"/>
-    </row>
-    <row r="22" spans="2:21">
-      <c r="N22" s="36">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21">
-      <c r="N23" s="36">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21">
-      <c r="N24" s="36">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:21">
-      <c r="N25" s="36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:21">
-      <c r="N26" s="36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="2:21">
-      <c r="N27" s="36">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21">
-      <c r="N28" s="36">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="2:21">
-      <c r="N29" s="36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:21">
-      <c r="N30" s="37">
-        <v>10</v>
+      <c r="K19" s="40">
+        <v>-163766.13347981332</v>
+      </c>
+      <c r="L19" s="40">
+        <v>5343.0296195821938</v>
+      </c>
+      <c r="M19" s="40">
+        <v>-30.650425908104783</v>
+      </c>
+      <c r="N19" s="40">
+        <v>6.7504007346907174E-6</v>
+      </c>
+      <c r="O19" s="40">
+        <v>-178600.76191402914</v>
+      </c>
+      <c r="P19" s="40">
+        <v>-148931.5050455975</v>
+      </c>
+      <c r="Q19" s="40">
+        <v>-178600.76191402914</v>
+      </c>
+      <c r="R19" s="40">
+        <v>-148931.5050455975</v>
+      </c>
+    </row>
+    <row r="20" spans="10:18" ht="15.75" thickBot="1">
+      <c r="J20" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="K20" s="44">
+        <v>84.910189508376845</v>
+      </c>
+      <c r="L20" s="44">
+        <v>2.6752709074016283</v>
+      </c>
+      <c r="M20" s="44">
+        <v>31.738912598891279</v>
+      </c>
+      <c r="N20" s="44">
+        <v>5.873735477721972E-6</v>
+      </c>
+      <c r="O20" s="44">
+        <v>77.482446692443531</v>
+      </c>
+      <c r="P20" s="44">
+        <v>92.33793232431016</v>
+      </c>
+      <c r="Q20" s="44">
+        <v>77.482446692443531</v>
+      </c>
+      <c r="R20" s="44">
+        <v>92.33793232431016</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="T19:U19"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3054,13 +2997,13 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="74"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="66"/>
       <c r="K5" t="s">
         <v>15</v>
       </c>
@@ -3091,13 +3034,13 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="4"/>
-      <c r="K7" s="69" t="s">
+      <c r="K7" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="70"/>
-      <c r="M7" s="70"/>
-      <c r="N7" s="70"/>
-      <c r="O7" s="71"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="63"/>
     </row>
     <row r="8" spans="1:15">
       <c r="B8" s="3"/>
@@ -3328,11 +3271,11 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="11" t="s">
@@ -3397,11 +3340,11 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="77"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="69"/>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" s="11" t="s">
@@ -3489,11 +3432,11 @@
       <c r="A28" s="16"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="76"/>
-      <c r="D29" s="77"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="69"/>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="11" t="s">
@@ -3613,11 +3556,11 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="77"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="69"/>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="11" t="s">
@@ -3658,11 +3601,11 @@
       <c r="A11" s="16"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="61"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="53"/>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="11" t="s">
@@ -3709,11 +3652,11 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="64"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="56"/>
     </row>
     <row r="22" spans="1:4">
       <c r="B22" s="11" t="s">
@@ -3798,11 +3741,11 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="B35" s="65" t="s">
+      <c r="B35" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="67"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="59"/>
     </row>
     <row r="36" spans="1:4">
       <c r="B36" s="11" t="s">
@@ -3882,11 +3825,11 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="B48" s="78" t="s">
+      <c r="B48" s="70" t="s">
         <v>128</v>
       </c>
-      <c r="C48" s="79"/>
-      <c r="D48" s="80"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="72"/>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" s="11" t="s">
@@ -3996,23 +3939,23 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="F5" s="81" t="s">
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="F5" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="K5" s="81" t="s">
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="K5" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
     </row>
     <row r="6" spans="1:15">
       <c r="B6" t="s">
@@ -4120,19 +4063,19 @@
         <f>_xlfn.NORM.S.INV(1-C10/2)</f>
         <v>1.9599639845400536</v>
       </c>
-      <c r="K10" s="81" t="s">
+      <c r="K10" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="F11" s="81" t="s">
+      <c r="F11" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
       <c r="I11" s="33"/>
       <c r="K11" t="s">
         <v>142</v>
@@ -4147,9 +4090,9 @@
       <c r="I12" s="34"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="16" t="s">
@@ -4173,22 +4116,22 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="F20" s="81" t="s">
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="F20" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
-      <c r="K20" s="81" t="s">
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="K20" s="73" t="s">
         <v>167</v>
       </c>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="81"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
     </row>
     <row r="21" spans="1:14">
       <c r="B21" s="19" t="s">
@@ -4312,35 +4255,40 @@
         <f>_xlfn.T.INV(1-D22/2,D21-1)</f>
         <v>3.1824463052837078</v>
       </c>
-      <c r="K25" s="81" t="s">
+      <c r="K25" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="L25" s="81"/>
-      <c r="M25" s="81"/>
-      <c r="N25" s="81"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="73"/>
+      <c r="N25" s="73"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="F26" s="81" t="s">
+      <c r="F26" s="73" t="s">
         <v>165</v>
       </c>
-      <c r="G26" s="81"/>
-      <c r="H26" s="81"/>
-      <c r="K26" s="81" t="s">
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="K26" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="L26" s="81"/>
-      <c r="M26" s="81"/>
-      <c r="N26" s="81"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="73"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="F27" s="81" t="s">
+      <c r="F27" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="G27" s="81"/>
-      <c r="H27" s="81"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K25:N25"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="K5:O5"/>
     <mergeCell ref="K10:N10"/>
@@ -4349,11 +4297,6 @@
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K25:N25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4384,11 +4327,11 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
     </row>
     <row r="7" spans="1:9">
       <c r="B7" t="s">
@@ -4453,13 +4396,13 @@
         <f>8/48</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E11" s="81" t="s">
+      <c r="E11" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
     </row>
     <row r="12" spans="1:9">
       <c r="E12" t="s">
@@ -4477,11 +4420,11 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
     </row>
     <row r="20" spans="1:9">
       <c r="B20" t="s">
@@ -4547,13 +4490,13 @@
         <f>6/50</f>
         <v>0.12</v>
       </c>
-      <c r="E24" s="81" t="s">
+      <c r="E24" s="73" t="s">
         <v>184</v>
       </c>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="81"/>
-      <c r="I24" s="81"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
     </row>
     <row r="25" spans="1:9">
       <c r="E25" t="s">
@@ -4600,11 +4543,11 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
     </row>
     <row r="9" spans="1:12">
       <c r="C9" t="s">
@@ -4668,31 +4611,31 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="73" t="s">
         <v>195</v>
       </c>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="F14" s="81" t="s">
+      <c r="F14" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="73"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="F15" s="81" t="s">
+      <c r="F15" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4724,14 +4667,14 @@
       </c>
     </row>
     <row r="4" spans="2:30">
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81" t="s">
+      <c r="C4" s="73"/>
+      <c r="D4" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="E4" s="81"/>
+      <c r="E4" s="73"/>
       <c r="G4" s="16" t="s">
         <v>200</v>
       </c>
@@ -4766,10 +4709,10 @@
       <c r="E6">
         <v>56</v>
       </c>
-      <c r="G6" s="81" t="s">
+      <c r="G6" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="H6" s="81"/>
+      <c r="H6" s="73"/>
       <c r="I6" t="s">
         <v>206</v>
       </c>
@@ -5266,795 +5209,984 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F320105-7FE0-43B3-B420-835C44619676}">
-  <dimension ref="B2:S41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8BFC71-637A-402C-908B-044747BF6BC6}">
+  <dimension ref="B2:AA52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="J32" workbookViewId="0">
+      <selection activeCell="W53" sqref="W53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="22" max="22" width="6" customWidth="1"/>
+    <col min="23" max="23" width="20.140625" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.85546875" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
-      <c r="B2" s="43" t="s">
+    <row r="2" spans="2:27">
+      <c r="B2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27">
+      <c r="B3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27">
+      <c r="C5" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="H5" s="77" t="s">
+        <v>251</v>
+      </c>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="N5" s="77" t="s">
+        <v>259</v>
+      </c>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="Y5" s="77" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z5" s="77"/>
+      <c r="AA5" s="77"/>
+    </row>
+    <row r="6" spans="2:27">
+      <c r="C6" s="35">
+        <v>7</v>
+      </c>
+      <c r="D6" s="35">
+        <v>11</v>
+      </c>
+      <c r="E6" s="35">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>252</v>
+      </c>
+      <c r="N6" s="35">
+        <v>7</v>
+      </c>
+      <c r="P6" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q6">
+        <f>AVERAGE(N6:N30)</f>
+        <v>10.68</v>
+      </c>
+      <c r="X6" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y6" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z6" s="19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27">
+      <c r="C7" s="36">
+        <v>12</v>
+      </c>
+      <c r="D7" s="36">
+        <v>17</v>
+      </c>
+      <c r="E7" s="36">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>253</v>
+      </c>
+      <c r="N7" s="36">
+        <v>12</v>
+      </c>
+      <c r="P7" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q7">
+        <f>_xlfn.STDEV.S(N6:N30)</f>
+        <v>3.2496153618543846</v>
+      </c>
+      <c r="X7" s="35">
+        <v>7</v>
+      </c>
+      <c r="Y7" s="35">
+        <v>11</v>
+      </c>
+      <c r="Z7" s="35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27">
+      <c r="C8" s="36">
+        <v>9</v>
+      </c>
+      <c r="D8" s="36">
+        <v>16</v>
+      </c>
+      <c r="E8" s="36">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>235</v>
+      </c>
+      <c r="I8">
+        <f>D17/C17</f>
+        <v>2.5854037267080727</v>
+      </c>
+      <c r="N8" s="36">
+        <v>9</v>
+      </c>
+      <c r="P8" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q8">
+        <f>_xlfn.NORM.INV(0.16,$Q$6,$Q$7)</f>
+        <v>7.448394386004404</v>
+      </c>
+      <c r="X8" s="36">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="36">
+        <v>17</v>
+      </c>
+      <c r="Z8" s="36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27">
+      <c r="C9" s="36">
+        <v>11</v>
+      </c>
+      <c r="D9" s="36">
+        <v>13</v>
+      </c>
+      <c r="E9" s="36">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>254</v>
+      </c>
+      <c r="I9">
+        <f>_xlfn.F.INV(0.025,D18 - 1, C18 - 1)</f>
+        <v>0.20733049797574626</v>
+      </c>
+      <c r="N9" s="36">
+        <v>11</v>
+      </c>
+      <c r="P9" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q9">
+        <f>_xlfn.NORM.INV(0.16 + 0.17,$Q$6,$Q$7)</f>
+        <v>9.2504514189462661</v>
+      </c>
+      <c r="X9" s="36">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="36">
+        <v>16</v>
+      </c>
+      <c r="Z9" s="36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27">
+      <c r="C10" s="36">
+        <v>8</v>
+      </c>
+      <c r="D10" s="36">
+        <v>10</v>
+      </c>
+      <c r="E10" s="36">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>255</v>
+      </c>
+      <c r="I10">
+        <f>_xlfn.F.INV(1 - 0.025,D18 - 1, C18 - 1)</f>
+        <v>4.1970466369455171</v>
+      </c>
+      <c r="N10" s="36">
+        <v>8</v>
+      </c>
+      <c r="P10" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q10">
+        <f>_xlfn.NORM.INV(0.16 + 0.17*2,$Q$6,$Q$7)</f>
+        <v>10.68</v>
+      </c>
+      <c r="X10" s="36">
+        <v>11</v>
+      </c>
+      <c r="Y10" s="36">
+        <v>13</v>
+      </c>
+      <c r="Z10" s="36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27">
+      <c r="C11" s="36">
+        <v>9</v>
+      </c>
+      <c r="D11" s="36">
+        <v>15</v>
+      </c>
+      <c r="E11" s="36">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>256</v>
+      </c>
+      <c r="N11" s="36">
+        <v>9</v>
+      </c>
+      <c r="P11" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q11">
+        <f>_xlfn.NORM.INV(0.16 + 0.17*3,$Q$6,$Q$7)</f>
+        <v>12.109548581053733</v>
+      </c>
+      <c r="X11" s="36">
+        <v>8</v>
+      </c>
+      <c r="Y11" s="36">
+        <v>10</v>
+      </c>
+      <c r="Z11" s="36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27">
+      <c r="C12" s="36">
+        <v>11</v>
+      </c>
+      <c r="D12" s="36">
+        <v>14</v>
+      </c>
+      <c r="E12" s="36">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>257</v>
+      </c>
+      <c r="N12" s="36">
+        <v>11</v>
+      </c>
+      <c r="P12" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q12">
+        <f>_xlfn.NORM.INV(0.16 + 0.17*4,$Q$6,$Q$7)</f>
+        <v>13.911605613995604</v>
+      </c>
+      <c r="X12" s="36">
+        <v>9</v>
+      </c>
+      <c r="Y12" s="36">
+        <v>15</v>
+      </c>
+      <c r="Z12" s="36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27">
+      <c r="C13" s="36">
+        <v>10</v>
+      </c>
+      <c r="D13" s="36">
+        <v>18</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="H13" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="N13" s="36">
+        <v>10</v>
+      </c>
+      <c r="X13" s="36">
+        <v>11</v>
+      </c>
+      <c r="Y13" s="36">
+        <v>14</v>
+      </c>
+      <c r="Z13" s="36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27">
+      <c r="C14" s="36">
+        <v>7</v>
+      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="N14" s="36">
+        <v>7</v>
+      </c>
+      <c r="R14" t="s">
+        <v>267</v>
+      </c>
+      <c r="S14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T14" s="73" t="s">
+        <v>270</v>
+      </c>
+      <c r="U14" s="73"/>
+      <c r="V14" s="46"/>
+      <c r="X14" s="36">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="36">
+        <v>18</v>
+      </c>
+      <c r="Z14" s="36"/>
+    </row>
+    <row r="15" spans="2:27">
+      <c r="C15" s="37">
+        <v>8</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="N15" s="36">
+        <v>8</v>
+      </c>
+      <c r="P15" s="73" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q15" s="73"/>
+      <c r="R15">
+        <f>COUNTIF(N6:N30,"&lt;"&amp;Q8)</f>
+        <v>4</v>
+      </c>
+      <c r="S15">
+        <f>D19*0.16</f>
+        <v>4</v>
+      </c>
+      <c r="T15" s="73">
+        <f>(R15-S15)^2/S15</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="73"/>
+      <c r="V15" s="46"/>
+      <c r="X15" s="36">
+        <v>7</v>
+      </c>
+      <c r="Y15" s="36"/>
+      <c r="Z15" s="36"/>
+    </row>
+    <row r="16" spans="2:27">
+      <c r="N16" s="36">
+        <v>11</v>
+      </c>
+      <c r="P16" s="73" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q16" s="73"/>
+      <c r="R16">
+        <f>COUNTIFS($N$6:$N$30,"&gt;"&amp;Q8,$N$6:$N$30,"&lt;"&amp;Q9)</f>
+        <v>6</v>
+      </c>
+      <c r="S16">
+        <f>$D$19*0.17</f>
+        <v>4.25</v>
+      </c>
+      <c r="T16" s="73">
+        <f t="shared" ref="T16:T20" si="0">(R16-S16)^2/S16</f>
+        <v>0.72058823529411764</v>
+      </c>
+      <c r="U16" s="73"/>
+      <c r="V16" s="46"/>
+      <c r="X16" s="37">
+        <v>8</v>
+      </c>
+      <c r="Y16" s="37"/>
+      <c r="Z16" s="37"/>
+    </row>
+    <row r="17" spans="2:26">
+      <c r="B17" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17">
+        <f>_xlfn.VAR.S(C6:C15)</f>
+        <v>3.0666666666666691</v>
+      </c>
+      <c r="D17">
+        <f>_xlfn.VAR.S(D6:D13)</f>
+        <v>7.9285714285714288</v>
+      </c>
+      <c r="E17">
+        <f>_xlfn.VAR.S(E6:E12)</f>
+        <v>3.2380952380952408</v>
+      </c>
+      <c r="N17" s="36">
+        <v>17</v>
+      </c>
+      <c r="P17" s="73" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q17" s="73"/>
+      <c r="R17">
+        <f t="shared" ref="R17:R19" si="1">COUNTIFS($N$6:$N$30,"&gt;"&amp;Q9,$N$6:$N$30,"&lt;"&amp;Q10)</f>
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <f t="shared" ref="S17:S19" si="2">$D$19*0.17</f>
+        <v>4.25</v>
+      </c>
+      <c r="T17" s="73">
+        <f t="shared" si="0"/>
+        <v>1.4705882352941176E-2</v>
+      </c>
+      <c r="U17" s="73"/>
+      <c r="V17" s="46"/>
+      <c r="W17" t="s">
         <v>231</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-    </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="43" t="s">
+      <c r="X17">
+        <f>AVERAGE(X7:X16)</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="Y17">
+        <f>AVERAGE(Y7:Y14)</f>
+        <v>14.25</v>
+      </c>
+      <c r="Z17">
+        <f>AVERAGE(Z7:Z13)</f>
+        <v>8.7142857142857135</v>
+      </c>
+    </row>
+    <row r="18" spans="2:26">
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18">
+        <f>COUNT(C6:C15)</f>
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:E18" si="3">COUNT(D6:D15)</f>
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="N18" s="36">
+        <v>16</v>
+      </c>
+      <c r="P18" s="73" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q18" s="73"/>
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="2"/>
+        <v>4.25</v>
+      </c>
+      <c r="T18" s="73">
+        <f t="shared" si="0"/>
+        <v>0.13235294117647059</v>
+      </c>
+      <c r="U18" s="73"/>
+      <c r="V18" s="46"/>
+      <c r="W18" t="s">
+        <v>279</v>
+      </c>
+      <c r="X18">
+        <f>AVERAGE(X7:Z16)</f>
+        <v>10.68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:26">
+      <c r="B19" s="73" t="s">
+        <v>269</v>
+      </c>
+      <c r="C19" s="73"/>
+      <c r="D19">
+        <f>SUM(C18:E18)</f>
+        <v>25</v>
+      </c>
+      <c r="N19" s="36">
+        <v>13</v>
+      </c>
+      <c r="P19" s="73" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q19" s="73"/>
+      <c r="R19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="2"/>
+        <v>4.25</v>
+      </c>
+      <c r="T19" s="73">
+        <f t="shared" si="0"/>
+        <v>2.4852941176470589</v>
+      </c>
+      <c r="U19" s="73"/>
+      <c r="V19" s="46"/>
+    </row>
+    <row r="20" spans="2:26">
+      <c r="N20" s="36">
+        <v>10</v>
+      </c>
+      <c r="P20" s="73" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q20" s="73"/>
+      <c r="R20">
+        <f>COUNTIF(N6:N30,"&gt;"&amp;Q12)</f>
+        <v>5</v>
+      </c>
+      <c r="S20">
+        <f>D19*0.16</f>
+        <v>4</v>
+      </c>
+      <c r="T20" s="73">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="U20" s="73"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="X20" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y20" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z20" s="19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="21" spans="2:26">
+      <c r="N21" s="36">
+        <v>15</v>
+      </c>
+      <c r="R21" s="77" t="s">
+        <v>277</v>
+      </c>
+      <c r="S21" s="77"/>
+      <c r="T21" s="77">
+        <f>SUM(T15:U20)</f>
+        <v>3.6029411764705883</v>
+      </c>
+      <c r="U21" s="77"/>
+      <c r="V21" s="47"/>
+      <c r="X21" s="36">
+        <f>X7-$X$17</f>
+        <v>-2.1999999999999993</v>
+      </c>
+      <c r="Y21" s="35">
+        <f>Y7-$Y$17</f>
+        <v>-3.25</v>
+      </c>
+      <c r="Z21" s="35">
+        <f>Z7-$Z$17</f>
+        <v>-0.71428571428571352</v>
+      </c>
+    </row>
+    <row r="22" spans="2:26">
+      <c r="N22" s="36">
+        <v>14</v>
+      </c>
+      <c r="X22" s="36">
+        <f t="shared" ref="X22:X30" si="4">X8-$X$17</f>
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="Y22" s="36">
+        <f t="shared" ref="Y22:Y28" si="5">Y8-$Y$17</f>
+        <v>2.75</v>
+      </c>
+      <c r="Z22" s="36">
+        <f t="shared" ref="Z22:Z27" si="6">Z8-$Z$17</f>
+        <v>-2.7142857142857135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:26">
+      <c r="N23" s="36">
+        <v>18</v>
+      </c>
+      <c r="X23" s="36">
+        <f t="shared" si="4"/>
+        <v>-0.19999999999999929</v>
+      </c>
+      <c r="Y23" s="36">
+        <f t="shared" si="5"/>
+        <v>1.75</v>
+      </c>
+      <c r="Z23" s="36">
+        <f t="shared" si="6"/>
+        <v>1.2857142857142865</v>
+      </c>
+    </row>
+    <row r="24" spans="2:26">
+      <c r="N24" s="36">
+        <v>8</v>
+      </c>
+      <c r="X24" s="36">
+        <f t="shared" si="4"/>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="Y24" s="36">
+        <f t="shared" si="5"/>
+        <v>-1.25</v>
+      </c>
+      <c r="Z24" s="36">
+        <f t="shared" si="6"/>
+        <v>0.28571428571428648</v>
+      </c>
+    </row>
+    <row r="25" spans="2:26">
+      <c r="N25" s="36">
+        <v>6</v>
+      </c>
+      <c r="X25" s="36">
+        <f t="shared" si="4"/>
+        <v>-1.1999999999999993</v>
+      </c>
+      <c r="Y25" s="36">
+        <f t="shared" si="5"/>
+        <v>-4.25</v>
+      </c>
+      <c r="Z25" s="36">
+        <f t="shared" si="6"/>
+        <v>2.2857142857142865</v>
+      </c>
+    </row>
+    <row r="26" spans="2:26">
+      <c r="N26" s="36">
+        <v>10</v>
+      </c>
+      <c r="X26" s="36">
+        <f t="shared" si="4"/>
+        <v>-0.19999999999999929</v>
+      </c>
+      <c r="Y26" s="36">
+        <f t="shared" si="5"/>
+        <v>0.75</v>
+      </c>
+      <c r="Z26" s="36">
+        <f t="shared" si="6"/>
+        <v>-1.7142857142857135</v>
+      </c>
+    </row>
+    <row r="27" spans="2:26">
+      <c r="N27" s="36">
+        <v>9</v>
+      </c>
+      <c r="X27" s="36">
+        <f t="shared" si="4"/>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="Y27" s="36">
+        <f t="shared" si="5"/>
+        <v>-0.25</v>
+      </c>
+      <c r="Z27" s="36">
+        <f t="shared" si="6"/>
+        <v>1.2857142857142865</v>
+      </c>
+    </row>
+    <row r="28" spans="2:26">
+      <c r="N28" s="36">
+        <v>11</v>
+      </c>
+      <c r="X28" s="36">
+        <f t="shared" si="4"/>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="Y28" s="36">
+        <f t="shared" si="5"/>
+        <v>3.75</v>
+      </c>
+      <c r="Z28" s="36"/>
+    </row>
+    <row r="29" spans="2:26">
+      <c r="N29" s="36">
+        <v>7</v>
+      </c>
+      <c r="X29" s="36">
+        <f t="shared" si="4"/>
+        <v>-2.1999999999999993</v>
+      </c>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="36"/>
+    </row>
+    <row r="30" spans="2:26">
+      <c r="N30" s="37">
+        <v>10</v>
+      </c>
+      <c r="X30" s="37">
+        <f t="shared" si="4"/>
+        <v>-1.1999999999999993</v>
+      </c>
+      <c r="Y30" s="37"/>
+      <c r="Z30" s="37"/>
+    </row>
+    <row r="32" spans="2:26">
+      <c r="W32" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="X32" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y32" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z32" s="19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="23:26">
+      <c r="X33" s="35">
+        <f>X21^2</f>
+        <v>4.8399999999999972</v>
+      </c>
+      <c r="Y33" s="35">
+        <f t="shared" ref="Y33:Z33" si="7">Y21^2</f>
+        <v>10.5625</v>
+      </c>
+      <c r="Z33" s="35">
+        <f t="shared" si="7"/>
+        <v>0.51020408163265196</v>
+      </c>
+    </row>
+    <row r="34" spans="23:26">
+      <c r="X34" s="36">
+        <f t="shared" ref="X34:Z42" si="8">X22^2</f>
+        <v>7.8400000000000043</v>
+      </c>
+      <c r="Y34" s="36">
+        <f t="shared" si="8"/>
+        <v>7.5625</v>
+      </c>
+      <c r="Z34" s="36">
+        <f t="shared" si="8"/>
+        <v>7.3673469387755057</v>
+      </c>
+    </row>
+    <row r="35" spans="23:26">
+      <c r="X35" s="36">
+        <f t="shared" si="8"/>
+        <v>3.9999999999999716E-2</v>
+      </c>
+      <c r="Y35" s="36">
+        <f t="shared" si="8"/>
+        <v>3.0625</v>
+      </c>
+      <c r="Z35" s="36">
+        <f t="shared" si="8"/>
+        <v>1.653061224489798</v>
+      </c>
+    </row>
+    <row r="36" spans="23:26">
+      <c r="X36" s="36">
+        <f t="shared" si="8"/>
+        <v>3.2400000000000024</v>
+      </c>
+      <c r="Y36" s="36">
+        <f t="shared" si="8"/>
+        <v>1.5625</v>
+      </c>
+      <c r="Z36" s="36">
+        <f t="shared" si="8"/>
+        <v>8.1632653061224927E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="23:26">
+      <c r="X37" s="36">
+        <f t="shared" si="8"/>
+        <v>1.4399999999999984</v>
+      </c>
+      <c r="Y37" s="36">
+        <f t="shared" si="8"/>
+        <v>18.0625</v>
+      </c>
+      <c r="Z37" s="36">
+        <f t="shared" si="8"/>
+        <v>5.2244897959183705</v>
+      </c>
+    </row>
+    <row r="38" spans="23:26">
+      <c r="X38" s="36">
+        <f t="shared" si="8"/>
+        <v>3.9999999999999716E-2</v>
+      </c>
+      <c r="Y38" s="36">
+        <f t="shared" si="8"/>
+        <v>0.5625</v>
+      </c>
+      <c r="Z38" s="36">
+        <f t="shared" si="8"/>
+        <v>2.9387755102040791</v>
+      </c>
+    </row>
+    <row r="39" spans="23:26">
+      <c r="X39" s="36">
+        <f t="shared" si="8"/>
+        <v>3.2400000000000024</v>
+      </c>
+      <c r="Y39" s="36">
+        <f t="shared" si="8"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="Z39" s="36">
+        <f t="shared" si="8"/>
+        <v>1.653061224489798</v>
+      </c>
+    </row>
+    <row r="40" spans="23:26">
+      <c r="X40" s="36">
+        <f t="shared" si="8"/>
+        <v>0.64000000000000112</v>
+      </c>
+      <c r="Y40" s="36">
+        <f t="shared" si="8"/>
+        <v>14.0625</v>
+      </c>
+      <c r="Z40" s="36"/>
+    </row>
+    <row r="41" spans="23:26">
+      <c r="X41" s="36">
+        <f t="shared" si="8"/>
+        <v>4.8399999999999972</v>
+      </c>
+      <c r="Y41" s="36"/>
+      <c r="Z41" s="36"/>
+    </row>
+    <row r="42" spans="23:26">
+      <c r="X42" s="37">
+        <f t="shared" si="8"/>
+        <v>1.4399999999999984</v>
+      </c>
+      <c r="Y42" s="37"/>
+      <c r="Z42" s="37"/>
+    </row>
+    <row r="43" spans="23:26">
+      <c r="W43" t="s">
+        <v>282</v>
+      </c>
+      <c r="X43" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="44" spans="23:26">
+      <c r="W44" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="X44" s="16">
+        <f>SUM(X33:Z42)</f>
+        <v>102.52857142857147</v>
+      </c>
+    </row>
+    <row r="45" spans="23:26">
+      <c r="W45" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="X45" s="16">
+        <f>X44/(25-3)</f>
+        <v>4.6603896103896121</v>
+      </c>
+    </row>
+    <row r="46" spans="23:26">
+      <c r="W46" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="43" t="s">
-        <v>233</v>
-      </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" s="43" t="s">
-        <v>232</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="51" t="s">
-        <v>235</v>
-      </c>
-      <c r="C7" s="85" t="s">
-        <v>240</v>
-      </c>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="43"/>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="51" t="s">
+      <c r="X46" s="16">
+        <f>10*(X17-X18)^2 + 8*(Y17-X18)^2 + 7*(Z17-X18)^2</f>
+        <v>150.91142857142862</v>
+      </c>
+    </row>
+    <row r="47" spans="23:26">
+      <c r="W47" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="X47" s="16">
+        <f>X46/(3-1)</f>
+        <v>75.455714285714308</v>
+      </c>
+    </row>
+    <row r="48" spans="23:26">
+      <c r="W48" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="X48" s="16">
+        <f>X47/X45</f>
+        <v>16.190859690678554</v>
+      </c>
+    </row>
+    <row r="49" spans="23:24">
+      <c r="W49" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="X49" s="16">
+        <f>_xlfn.F.INV(0.95,3-1,25-3)</f>
+        <v>3.4433567793667228</v>
+      </c>
+    </row>
+    <row r="50" spans="23:24">
+      <c r="W50" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="C8" s="46">
-        <v>45</v>
-      </c>
-      <c r="D8" s="46">
-        <v>59</v>
-      </c>
-      <c r="E8" s="46">
-        <v>48</v>
-      </c>
-      <c r="F8" s="46">
-        <v>46</v>
-      </c>
-      <c r="G8" s="46">
-        <v>38</v>
-      </c>
-      <c r="H8" s="47">
-        <v>47</v>
-      </c>
-      <c r="J8">
-        <f>_xlfn.VAR.S(C8:H8)</f>
-        <v>46.166666666666785</v>
-      </c>
-      <c r="K8">
-        <f>J10/J9</f>
-        <v>8.8825301204819382</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="51" t="s">
+    </row>
+    <row r="51" spans="23:24">
+      <c r="W51" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="C9" s="49">
-        <v>21</v>
-      </c>
-      <c r="D9" s="49">
-        <v>12</v>
-      </c>
-      <c r="E9" s="49">
-        <v>14</v>
-      </c>
-      <c r="F9" s="49">
-        <v>17</v>
-      </c>
-      <c r="G9" s="49">
-        <v>13</v>
-      </c>
-      <c r="H9" s="50">
-        <v>17</v>
-      </c>
-      <c r="J9">
-        <f t="shared" ref="J9:J11" si="0">_xlfn.VAR.S(C9:H9)</f>
-        <v>11.066666666666652</v>
-      </c>
-      <c r="K9">
-        <f>_xlfn.F.INV(0.025,5,5)</f>
-        <v>0.13993095022986143</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="51" t="s">
-        <v>238</v>
-      </c>
-      <c r="C10" s="49">
-        <v>37</v>
-      </c>
-      <c r="D10" s="49">
-        <v>32</v>
-      </c>
-      <c r="E10" s="49">
-        <v>15</v>
-      </c>
-      <c r="F10" s="49">
-        <v>25</v>
-      </c>
-      <c r="G10" s="49">
-        <v>39</v>
-      </c>
-      <c r="H10" s="50">
-        <v>41</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>98.3</v>
-      </c>
-      <c r="K10">
-        <f>_xlfn.F.INV(0.975,5,5)</f>
-        <v>7.1463818287328316</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="B11" s="51" t="s">
-        <v>239</v>
-      </c>
-      <c r="C11" s="49">
-        <v>16</v>
-      </c>
-      <c r="D11" s="49">
-        <v>11</v>
-      </c>
-      <c r="E11" s="49">
-        <v>20</v>
-      </c>
-      <c r="F11" s="49">
-        <v>21</v>
-      </c>
-      <c r="G11" s="49">
-        <v>14</v>
-      </c>
-      <c r="H11" s="50">
-        <v>7</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>28.566666666666652</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11">
-      <c r="B15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11">
-      <c r="B16" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19">
-      <c r="C18" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="M18" s="19" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19">
-      <c r="B19" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="C19" s="48">
-        <f>AVERAGE(C8:H8)</f>
-        <v>47.166666666666664</v>
-      </c>
-      <c r="E19" s="45" t="s">
-        <v>247</v>
-      </c>
-      <c r="F19" s="45">
-        <f>C8-$C$19</f>
-        <v>-2.1666666666666643</v>
-      </c>
-      <c r="G19" s="46">
-        <f t="shared" ref="G19:J19" si="1">D8-$C$19</f>
-        <v>11.833333333333336</v>
-      </c>
-      <c r="H19" s="46">
-        <f t="shared" si="1"/>
-        <v>0.8333333333333357</v>
-      </c>
-      <c r="I19" s="46">
-        <f t="shared" si="1"/>
-        <v>-1.1666666666666643</v>
-      </c>
-      <c r="J19" s="46">
-        <f t="shared" si="1"/>
-        <v>-9.1666666666666643</v>
-      </c>
-      <c r="K19" s="47">
-        <f>H8-$C$19</f>
-        <v>-0.1666666666666643</v>
-      </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="N19" s="45">
-        <f t="shared" ref="N19:R22" si="2">F19^2</f>
-        <v>4.694444444444434</v>
-      </c>
-      <c r="O19" s="46">
-        <f t="shared" si="2"/>
-        <v>140.02777777777783</v>
-      </c>
-      <c r="P19" s="46">
-        <f t="shared" si="2"/>
-        <v>0.69444444444444842</v>
-      </c>
-      <c r="Q19" s="46">
-        <f t="shared" si="2"/>
-        <v>1.3611111111111056</v>
-      </c>
-      <c r="R19" s="46">
-        <f t="shared" si="2"/>
-        <v>84.027777777777729</v>
-      </c>
-      <c r="S19" s="47">
-        <f t="shared" ref="S19:S22" si="3">K19^2</f>
-        <v>2.7777777777776989E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19">
-      <c r="B20" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="C20" s="48">
-        <f>AVERAGE(C9:H9)</f>
-        <v>15.666666666666666</v>
-      </c>
-      <c r="E20" s="45" t="s">
-        <v>245</v>
-      </c>
-      <c r="F20" s="45">
-        <f>C9-$C$20</f>
-        <v>5.3333333333333339</v>
-      </c>
-      <c r="G20" s="46">
-        <f t="shared" ref="G20:J20" si="4">D9-$C$20</f>
-        <v>-3.6666666666666661</v>
-      </c>
-      <c r="H20" s="46">
-        <f t="shared" si="4"/>
-        <v>-1.6666666666666661</v>
-      </c>
-      <c r="I20" s="46">
-        <f t="shared" si="4"/>
-        <v>1.3333333333333339</v>
-      </c>
-      <c r="J20" s="46">
-        <f t="shared" si="4"/>
-        <v>-2.6666666666666661</v>
-      </c>
-      <c r="K20" s="47">
-        <f>H9-$C$20</f>
-        <v>1.3333333333333339</v>
-      </c>
-      <c r="L20" s="1"/>
-      <c r="M20" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="N20" s="45">
-        <f t="shared" si="2"/>
-        <v>28.44444444444445</v>
-      </c>
-      <c r="O20" s="46">
-        <f t="shared" si="2"/>
-        <v>13.444444444444439</v>
-      </c>
-      <c r="P20" s="46">
-        <f t="shared" si="2"/>
-        <v>2.7777777777777759</v>
-      </c>
-      <c r="Q20" s="46">
-        <f t="shared" si="2"/>
-        <v>1.7777777777777795</v>
-      </c>
-      <c r="R20" s="46">
-        <f t="shared" si="2"/>
-        <v>7.1111111111111081</v>
-      </c>
-      <c r="S20" s="47">
-        <f t="shared" si="3"/>
-        <v>1.7777777777777795</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19">
-      <c r="B21" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="C21" s="48">
-        <f t="shared" ref="C21:C22" si="5">AVERAGE(C10:H10)</f>
-        <v>31.5</v>
-      </c>
-      <c r="E21" s="45" t="s">
-        <v>246</v>
-      </c>
-      <c r="F21" s="45">
-        <f>C10-$C$21</f>
-        <v>5.5</v>
-      </c>
-      <c r="G21" s="46">
-        <f t="shared" ref="G21:J21" si="6">D10-$C$21</f>
-        <v>0.5</v>
-      </c>
-      <c r="H21" s="46">
-        <f t="shared" si="6"/>
-        <v>-16.5</v>
-      </c>
-      <c r="I21" s="46">
-        <f t="shared" si="6"/>
-        <v>-6.5</v>
-      </c>
-      <c r="J21" s="46">
-        <f t="shared" si="6"/>
-        <v>7.5</v>
-      </c>
-      <c r="K21" s="47">
-        <f>H10-$C$21</f>
-        <v>9.5</v>
-      </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="N21" s="11">
-        <f t="shared" si="2"/>
-        <v>30.25</v>
-      </c>
-      <c r="O21" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="P21" s="1">
-        <f t="shared" si="2"/>
-        <v>272.25</v>
-      </c>
-      <c r="Q21" s="1">
-        <f t="shared" si="2"/>
-        <v>42.25</v>
-      </c>
-      <c r="R21" s="1">
-        <f t="shared" si="2"/>
-        <v>56.25</v>
-      </c>
-      <c r="S21" s="12">
-        <f t="shared" si="3"/>
-        <v>90.25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19">
-      <c r="B22" s="37" t="s">
-        <v>239</v>
-      </c>
-      <c r="C22" s="44">
-        <f t="shared" si="5"/>
-        <v>14.833333333333334</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="F22" s="13">
-        <f>C11-$C$22</f>
-        <v>1.1666666666666661</v>
-      </c>
-      <c r="G22" s="14">
-        <f t="shared" ref="G22:J22" si="7">D11-$C$22</f>
-        <v>-3.8333333333333339</v>
-      </c>
-      <c r="H22" s="14">
-        <f t="shared" si="7"/>
-        <v>5.1666666666666661</v>
-      </c>
-      <c r="I22" s="14">
-        <f t="shared" si="7"/>
-        <v>6.1666666666666661</v>
-      </c>
-      <c r="J22" s="14">
-        <f t="shared" si="7"/>
-        <v>-0.83333333333333393</v>
-      </c>
-      <c r="K22" s="15">
-        <f>H11-$C$22</f>
-        <v>-7.8333333333333339</v>
-      </c>
-      <c r="L22" s="1"/>
-      <c r="M22" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="N22" s="45">
-        <f t="shared" si="2"/>
-        <v>1.3611111111111098</v>
-      </c>
-      <c r="O22" s="46">
-        <f t="shared" si="2"/>
-        <v>14.694444444444448</v>
-      </c>
-      <c r="P22" s="46">
-        <f t="shared" si="2"/>
-        <v>26.694444444444439</v>
-      </c>
-      <c r="Q22" s="46">
-        <f t="shared" si="2"/>
-        <v>38.027777777777771</v>
-      </c>
-      <c r="R22" s="46">
-        <f t="shared" si="2"/>
-        <v>0.69444444444444542</v>
-      </c>
-      <c r="S22" s="47">
-        <f t="shared" si="3"/>
-        <v>61.361111111111121</v>
-      </c>
-    </row>
-    <row r="24" spans="2:19">
-      <c r="B24" t="s">
-        <v>250</v>
-      </c>
-      <c r="C24" s="52">
-        <f>AVERAGE(C8:H11)</f>
-        <v>27.291666666666668</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19">
-      <c r="C25" s="52"/>
-    </row>
-    <row r="26" spans="2:19">
-      <c r="B26" t="s">
-        <v>253</v>
-      </c>
-      <c r="C26" s="52">
-        <f>COUNT(C8:H11)</f>
-        <v>24</v>
-      </c>
-      <c r="E26" s="45" t="s">
-        <v>256</v>
-      </c>
-      <c r="F26" s="47">
-        <f>COUNT(C8:H8)</f>
-        <v>6</v>
-      </c>
-      <c r="H26" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19">
-      <c r="B27" t="s">
-        <v>254</v>
-      </c>
-      <c r="C27" s="16">
-        <f>4</f>
-        <v>4</v>
-      </c>
-      <c r="E27" s="45" t="s">
-        <v>257</v>
-      </c>
-      <c r="F27" s="47">
-        <f t="shared" ref="F27:F29" si="8">COUNT(C9:H9)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B28" t="s">
-        <v>251</v>
-      </c>
-      <c r="C28" s="16">
-        <f>SUM(N19:S22)</f>
-        <v>920.49999999999989</v>
-      </c>
-      <c r="E28" s="45" t="s">
-        <v>258</v>
-      </c>
-      <c r="F28" s="47">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="H28" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19">
-      <c r="B29" t="s">
-        <v>252</v>
-      </c>
-      <c r="C29" s="16">
-        <f>C28/(C26-C27)</f>
-        <v>46.024999999999991</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="F29" s="15">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="H29" s="54" t="s">
-        <v>268</v>
-      </c>
-      <c r="I29" s="54" t="s">
-        <v>269</v>
-      </c>
-      <c r="J29" s="54" t="s">
-        <v>270</v>
-      </c>
-      <c r="K29" s="54" t="s">
-        <v>244</v>
-      </c>
-      <c r="L29" s="54" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19">
-      <c r="B30" t="s">
-        <v>255</v>
-      </c>
-      <c r="C30" s="16">
-        <f>F26*(C19-C24)^2 + F27*(C20-C24)^2 + F28*(C21-C24)^2 + F29*(C22-C24)^2</f>
-        <v>4218.4583333333321</v>
-      </c>
-      <c r="H30" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="I30" s="40">
-        <v>6</v>
-      </c>
-      <c r="J30" s="40">
-        <v>283</v>
-      </c>
-      <c r="K30" s="40">
-        <v>47.166666666666664</v>
-      </c>
-      <c r="L30" s="40">
-        <v>46.166666666666785</v>
-      </c>
-    </row>
-    <row r="31" spans="2:19">
-      <c r="B31" t="s">
-        <v>260</v>
-      </c>
-      <c r="C31" s="16">
-        <f xml:space="preserve"> C30/(C27-1)</f>
-        <v>1406.1527777777774</v>
-      </c>
-      <c r="H31" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="I31" s="40">
-        <v>6</v>
-      </c>
-      <c r="J31" s="40">
-        <v>94</v>
-      </c>
-      <c r="K31" s="40">
-        <v>15.666666666666666</v>
-      </c>
-      <c r="L31" s="40">
-        <v>11.066666666666652</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19">
-      <c r="B32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C32" s="16">
-        <f>C31/C29</f>
-        <v>30.551934335204294</v>
-      </c>
-      <c r="H32" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="I32" s="40">
-        <v>6</v>
-      </c>
-      <c r="J32" s="40">
-        <v>189</v>
-      </c>
-      <c r="K32" s="40">
-        <v>31.5</v>
-      </c>
-      <c r="L32" s="40">
-        <v>98.3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B33" t="s">
-        <v>262</v>
-      </c>
-      <c r="C33" s="16">
-        <f xml:space="preserve"> _xlfn.F.INV(1 - 0.05, C27-1,C26-C27)</f>
-        <v>3.0983912121407773</v>
-      </c>
-      <c r="H33" s="53" t="s">
-        <v>239</v>
-      </c>
-      <c r="I33" s="53">
-        <v>6</v>
-      </c>
-      <c r="J33" s="53">
-        <v>89</v>
-      </c>
-      <c r="K33" s="53">
-        <v>14.833333333333334</v>
-      </c>
-      <c r="L33" s="53">
-        <v>28.566666666666652</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14">
-      <c r="B34" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14">
-      <c r="B35" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B36" t="s">
-        <v>265</v>
-      </c>
-      <c r="H36" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14">
-      <c r="H37" s="54" t="s">
-        <v>273</v>
-      </c>
-      <c r="I37" s="54" t="s">
-        <v>274</v>
-      </c>
-      <c r="J37" s="54" t="s">
-        <v>275</v>
-      </c>
-      <c r="K37" s="54" t="s">
-        <v>276</v>
-      </c>
-      <c r="L37" s="54" t="s">
-        <v>277</v>
-      </c>
-      <c r="M37" s="54" t="s">
-        <v>278</v>
-      </c>
-      <c r="N37" s="54" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14">
-      <c r="H38" s="40" t="s">
-        <v>280</v>
-      </c>
-      <c r="I38" s="55">
-        <v>4218.458333333333</v>
-      </c>
-      <c r="J38" s="40">
-        <v>3</v>
-      </c>
-      <c r="K38" s="55">
-        <v>1406.1527777777776</v>
-      </c>
-      <c r="L38" s="55">
-        <v>30.551934335204294</v>
-      </c>
-      <c r="M38" s="40">
-        <v>1.1510461331325205E-7</v>
-      </c>
-      <c r="N38" s="55">
-        <v>3.0983912121407795</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14">
-      <c r="H39" s="40" t="s">
-        <v>281</v>
-      </c>
-      <c r="I39" s="55">
-        <v>920.5</v>
-      </c>
-      <c r="J39" s="40">
-        <v>20</v>
-      </c>
-      <c r="K39" s="55">
-        <v>46.024999999999999</v>
-      </c>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-    </row>
-    <row r="40" spans="2:14">
-      <c r="H40" s="40"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="40"/>
-    </row>
-    <row r="41" spans="2:14" ht="15.75" thickBot="1">
-      <c r="H41" s="53" t="s">
-        <v>282</v>
-      </c>
-      <c r="I41" s="53">
-        <v>5138.958333333333</v>
-      </c>
-      <c r="J41" s="53">
-        <v>23</v>
-      </c>
-      <c r="K41" s="53"/>
-      <c r="L41" s="53"/>
-      <c r="M41" s="53"/>
-      <c r="N41" s="53"/>
+    </row>
+    <row r="52" spans="23:24">
+      <c r="W52" s="16" t="s">
+        <v>287</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C7:H7"/>
+  <mergeCells count="19">
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="R21:S21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>